<commit_message>
test fix in server print data fix of reports
</commit_message>
<xml_diff>
--- a/reporteRudel2.xlsx
+++ b/reporteRudel2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>Fabricación, Montaje, Mantención y Reparación</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Ito Planta Turno noche:</t>
+  </si>
+  <si>
+    <t>Victor Cortes</t>
   </si>
   <si>
     <t>Horas Programadas</t>
@@ -12902,7 +12905,7 @@
       <c r="AB12" s="23"/>
       <c r="AC12" s="23"/>
       <c r="AD12" s="24" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AE12" s="24"/>
       <c r="AF12" s="24"/>
@@ -13902,7 +13905,7 @@
     <row r="13" spans="1:1025" customHeight="1" ht="15">
       <c r="A13"/>
       <c r="B13" s="25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
@@ -13924,7 +13927,7 @@
       <c r="T13" s="25"/>
       <c r="U13" s="25"/>
       <c r="V13" s="26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="W13" s="26"/>
       <c r="X13" s="26"/>
@@ -14932,7 +14935,7 @@
     <row r="14" spans="1:1025" customHeight="1" ht="15">
       <c r="A14"/>
       <c r="B14" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -14941,7 +14944,7 @@
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
       <c r="I14" s="28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
@@ -14956,7 +14959,7 @@
       <c r="T14" s="28"/>
       <c r="U14" s="28"/>
       <c r="V14" s="29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W14" s="29"/>
       <c r="X14" s="29"/>
@@ -15964,7 +15967,7 @@
     <row r="15" spans="1:1025" customHeight="1" ht="15">
       <c r="A15"/>
       <c r="B15" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
@@ -15973,7 +15976,7 @@
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
       <c r="I15" s="28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
@@ -15988,7 +15991,7 @@
       <c r="T15" s="28"/>
       <c r="U15" s="28"/>
       <c r="V15" s="29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="W15" s="29"/>
       <c r="X15" s="29"/>
@@ -16996,7 +16999,7 @@
     <row r="16" spans="1:1025" customHeight="1" ht="15">
       <c r="A16"/>
       <c r="B16" s="32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
@@ -17018,7 +17021,7 @@
       <c r="T16" s="33"/>
       <c r="U16" s="33"/>
       <c r="V16" s="33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W16" s="33"/>
       <c r="X16" s="33"/>
@@ -18026,7 +18029,7 @@
     <row r="17" spans="1:1025" customHeight="1" ht="15">
       <c r="A17"/>
       <c r="B17" s="35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" s="35"/>
       <c r="D17" s="35"/>
@@ -20080,10 +20083,10 @@
     <row r="19" spans="1:1025" customHeight="1" ht="15">
       <c r="A19"/>
       <c r="B19" s="36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D19" s="37"/>
       <c r="E19" s="37"/>
@@ -20110,7 +20113,7 @@
       <c r="Z19" s="37"/>
       <c r="AA19" s="37"/>
       <c r="AB19" s="37" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AC19" s="37"/>
       <c r="AD19" s="37"/>
@@ -20118,7 +20121,7 @@
       <c r="AF19" s="37"/>
       <c r="AG19" s="37"/>
       <c r="AH19" s="37" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AI19" s="37"/>
       <c r="AJ19" s="37"/>
@@ -20126,7 +20129,7 @@
       <c r="AL19" s="37"/>
       <c r="AM19" s="37"/>
       <c r="AN19" s="38" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AO19" s="38"/>
       <c r="AP19" s="38"/>
@@ -42814,7 +42817,7 @@
     <row r="43" spans="1:1025" customHeight="1" ht="15">
       <c r="A43" s="10"/>
       <c r="B43" s="56" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C43" s="56"/>
       <c r="D43" s="56"/>
@@ -43842,7 +43845,7 @@
     <row r="44" spans="1:1025" customHeight="1" ht="15">
       <c r="A44" s="10"/>
       <c r="B44" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C44" s="25"/>
       <c r="D44" s="25"/>
@@ -43879,7 +43882,7 @@
       <c r="AI44" s="25"/>
       <c r="AJ44" s="25"/>
       <c r="AK44" s="26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AL44" s="26"/>
       <c r="AM44" s="26"/>
@@ -44873,7 +44876,7 @@
       <c r="A45" s="10"/>
       <c r="B45" s="57"/>
       <c r="C45" s="58" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D45" s="58"/>
       <c r="E45" s="58"/>
@@ -45901,7 +45904,7 @@
       <c r="A46" s="10"/>
       <c r="B46" s="57"/>
       <c r="C46" s="58" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D46" s="58"/>
       <c r="E46" s="58"/>
@@ -46929,7 +46932,7 @@
       <c r="A47" s="10"/>
       <c r="B47" s="62"/>
       <c r="C47" s="63" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D47" s="63"/>
       <c r="E47" s="63"/>
@@ -47956,7 +47959,7 @@
     <row r="48" spans="1:1025" customHeight="1" ht="15">
       <c r="A48" s="10"/>
       <c r="B48" s="66" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C48" s="66"/>
       <c r="D48" s="66"/>
@@ -48984,11 +48987,11 @@
     <row r="49" spans="1:1025" customHeight="1" ht="15">
       <c r="A49" s="10"/>
       <c r="B49" s="67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C49" s="67"/>
       <c r="D49" s="68" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E49" s="68"/>
       <c r="F49" s="68"/>
@@ -49002,11 +49005,11 @@
       <c r="N49" s="68"/>
       <c r="O49" s="68"/>
       <c r="P49" s="69" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q49" s="69"/>
       <c r="R49" s="68" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S49" s="68"/>
       <c r="T49" s="68"/>
@@ -49020,11 +49023,11 @@
       <c r="AB49" s="68"/>
       <c r="AC49" s="68"/>
       <c r="AD49" s="69" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE49" s="69"/>
       <c r="AF49" s="68" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AG49" s="68"/>
       <c r="AH49" s="68"/>
@@ -63404,11 +63407,11 @@
     <row r="64" spans="1:1025" customHeight="1" ht="15">
       <c r="A64"/>
       <c r="B64" s="67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C64" s="67"/>
       <c r="D64" s="68" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E64" s="68"/>
       <c r="F64" s="68"/>
@@ -63422,11 +63425,11 @@
       <c r="N64" s="68"/>
       <c r="O64" s="68"/>
       <c r="P64" s="69" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q64" s="69"/>
       <c r="R64" s="68" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S64" s="68"/>
       <c r="T64" s="68"/>
@@ -63440,11 +63443,11 @@
       <c r="AB64" s="68"/>
       <c r="AC64" s="68"/>
       <c r="AD64" s="69" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE64" s="69"/>
       <c r="AF64" s="75" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AG64" s="75"/>
       <c r="AH64" s="75"/>

</xml_diff>